<commit_message>
Committing changes related to extent reports and multi browser
</commit_message>
<xml_diff>
--- a/KeywordFramework_Grid_MultiBrowser/src/test/java/dataEngine/DataEngineN1C.xlsx
+++ b/KeywordFramework_Grid_MultiBrowser/src/test/java/dataEngine/DataEngineN1C.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79FEC06-82A5-4F76-A820-3E25859CFF94}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA46138-74FF-4525-A766-E5F2B3AB4801}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -273,7 +273,7 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Mozilla</t>
+    <t>Chrome</t>
   </si>
   <si>
     <t>PASS</t>
@@ -653,7 +653,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Framework improved for Mobile Automation
</commit_message>
<xml_diff>
--- a/KeywordFramework_Grid_MultiBrowser/src/test/java/dataEngine/DataEngineN1C.xlsx
+++ b/KeywordFramework_Grid_MultiBrowser/src/test/java/dataEngine/DataEngineN1C.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA46138-74FF-4525-A766-E5F2B3AB4801}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CBE56A-5764-464E-A1DE-8970F0906D5D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="80">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -283,8 +283,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,17 +652,17 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="45.453125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="26.90625" collapsed="true"/>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1062,7 +1061,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -1140,9 +1139,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="49.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1231,11 +1230,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.7265625" collapsed="true"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>